<commit_message>
20180403 in my office
</commit_message>
<xml_diff>
--- a/config/律师能力定级.xlsx
+++ b/config/律师能力定级.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9847" windowHeight="6120"/>
+    <workbookView windowWidth="18540" windowHeight="9730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>姓名</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>王彬</t>
+  </si>
+  <si>
+    <t>陈方圆</t>
   </si>
 </sst>
 </file>
@@ -80,9 +83,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -95,54 +98,53 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,51 +152,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,14 +166,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -224,6 +173,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -232,7 +197,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,13 +250,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,13 +328,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,25 +358,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,19 +388,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,97 +400,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,11 +444,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -466,16 +475,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,23 +503,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,8 +536,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,10 +549,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -558,133 +561,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,16 +1017,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.02727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="10.5929203539823"/>
-    <col min="3" max="3" width="11.3097345132743" customWidth="1"/>
+    <col min="2" max="2" width="10.5909090909091"/>
+    <col min="3" max="3" width="11.3090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1189,6 +1192,17 @@
       </c>
       <c r="C15" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42217</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1220,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.02727272727273" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1222,7 +1236,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.02727272727273" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>